<commit_message>
Added Facebook Pixel on every html page. Created Ad (for 2 days). Added a .txt file with all questions and answers, just for guidance.
</commit_message>
<xml_diff>
--- a/Color Mixtures/Color Blends.xlsx
+++ b/Color Mixtures/Color Blends.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulogarcia/Desktop/MEIC/blendingbox/Color Mixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PauloGarcia/Desktop/blendingbox/Color Mixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="8700" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Color Mixtures First Study" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="213">
   <si>
     <t>Cores a Misturar</t>
   </si>
@@ -661,6 +661,9 @@
   </si>
   <si>
     <t>#cbd7d1</t>
+  </si>
+  <si>
+    <t>#00A5FF</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="117">
+  <fills count="118">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1425,6 +1428,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A5FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1891,7 +1900,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2730,10 +2739,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="116" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2742,23 +2820,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2766,16 +2871,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2790,125 +2907,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="116" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="117" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2924,6 +2939,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF00A5FF"/>
       <color rgb="FFCBD7D1"/>
       <color rgb="FFF0AAD3"/>
       <color rgb="FFF0D5A3"/>
@@ -2933,7 +2949,6 @@
       <color rgb="FF80BFBF"/>
       <color rgb="FFBF80BF"/>
       <color rgb="FFBFBF80"/>
-      <color rgb="FF804040"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3308,7 +3323,7 @@
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
       <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="AB34" sqref="AB34"/>
+      <selection pane="topRight" activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3323,10 +3338,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="316" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="316"/>
+      <c r="B2" s="337" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="337"/>
       <c r="E2" t="s">
         <v>7</v>
       </c>
@@ -3509,10 +3524,10 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="321" t="s">
+      <c r="B10" s="343" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="321"/>
+      <c r="C10" s="343"/>
       <c r="D10" s="4">
         <v>0</v>
       </c>
@@ -3567,10 +3582,10 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="322" t="s">
+      <c r="B11" s="344" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="322"/>
+      <c r="C11" s="344"/>
       <c r="D11" s="4">
         <v>120</v>
       </c>
@@ -3625,10 +3640,10 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="323" t="s">
+      <c r="B12" s="345" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="323"/>
+      <c r="C12" s="345"/>
       <c r="D12" s="25">
         <v>240</v>
       </c>
@@ -3683,10 +3698,10 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="324" t="s">
+      <c r="B13" s="346" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="324"/>
+      <c r="C13" s="346"/>
       <c r="D13" s="4">
         <v>180</v>
       </c>
@@ -3741,10 +3756,10 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="325" t="s">
+      <c r="B14" s="347" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="325"/>
+      <c r="C14" s="347"/>
       <c r="D14" s="4">
         <v>300</v>
       </c>
@@ -3799,10 +3814,10 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="320" t="s">
+      <c r="B15" s="342" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="320"/>
+      <c r="C15" s="342"/>
       <c r="D15" s="6">
         <v>60</v>
       </c>
@@ -3858,52 +3873,52 @@
     </row>
     <row r="16" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:35" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="341" t="s">
+      <c r="B17" s="311" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="342"/>
-      <c r="D17" s="317" t="s">
+      <c r="C17" s="312"/>
+      <c r="D17" s="327" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="318"/>
-      <c r="F17" s="319"/>
-      <c r="G17" s="318" t="s">
+      <c r="E17" s="304"/>
+      <c r="F17" s="305"/>
+      <c r="G17" s="304" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="318"/>
-      <c r="I17" s="319"/>
-      <c r="J17" s="317" t="s">
+      <c r="H17" s="304"/>
+      <c r="I17" s="305"/>
+      <c r="J17" s="327" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="318"/>
-      <c r="L17" s="318"/>
-      <c r="M17" s="319"/>
-      <c r="N17" s="317" t="s">
+      <c r="K17" s="304"/>
+      <c r="L17" s="304"/>
+      <c r="M17" s="305"/>
+      <c r="N17" s="327" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="318"/>
-      <c r="P17" s="318"/>
-      <c r="Q17" s="333" t="s">
+      <c r="O17" s="304"/>
+      <c r="P17" s="304"/>
+      <c r="Q17" s="328" t="s">
         <v>91</v>
       </c>
-      <c r="R17" s="334"/>
-      <c r="S17" s="335"/>
-      <c r="T17" s="330" t="s">
+      <c r="R17" s="329"/>
+      <c r="S17" s="330"/>
+      <c r="T17" s="323" t="s">
         <v>51</v>
       </c>
-      <c r="U17" s="331"/>
-      <c r="V17" s="331"/>
-      <c r="W17" s="331"/>
-      <c r="X17" s="331"/>
-      <c r="Y17" s="331"/>
-      <c r="Z17" s="331"/>
-      <c r="AA17" s="331"/>
-      <c r="AB17" s="331"/>
-      <c r="AC17" s="332"/>
+      <c r="U17" s="324"/>
+      <c r="V17" s="324"/>
+      <c r="W17" s="324"/>
+      <c r="X17" s="324"/>
+      <c r="Y17" s="324"/>
+      <c r="Z17" s="324"/>
+      <c r="AA17" s="324"/>
+      <c r="AB17" s="324"/>
+      <c r="AC17" s="325"/>
     </row>
     <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="343"/>
-      <c r="C18" s="344"/>
+      <c r="B18" s="313"/>
+      <c r="C18" s="314"/>
       <c r="D18" s="22" t="s">
         <v>37</v>
       </c>
@@ -3952,32 +3967,32 @@
       <c r="S18" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="T18" s="336" t="s">
+      <c r="T18" s="331" t="s">
         <v>8</v>
       </c>
-      <c r="U18" s="337"/>
-      <c r="V18" s="338" t="s">
+      <c r="U18" s="332"/>
+      <c r="V18" s="333" t="s">
         <v>92</v>
       </c>
-      <c r="W18" s="337"/>
-      <c r="X18" s="338" t="s">
+      <c r="W18" s="332"/>
+      <c r="X18" s="333" t="s">
         <v>10</v>
       </c>
-      <c r="Y18" s="337"/>
-      <c r="Z18" s="338" t="s">
+      <c r="Y18" s="332"/>
+      <c r="Z18" s="333" t="s">
         <v>27</v>
       </c>
-      <c r="AA18" s="337"/>
-      <c r="AB18" s="339" t="s">
+      <c r="AA18" s="332"/>
+      <c r="AB18" s="334" t="s">
         <v>91</v>
       </c>
-      <c r="AC18" s="340"/>
+      <c r="AC18" s="335"/>
     </row>
     <row r="19" spans="1:35" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="347" t="s">
+      <c r="B19" s="319" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="348"/>
+      <c r="C19" s="320"/>
       <c r="D19" s="20">
         <v>60</v>
       </c>
@@ -4031,35 +4046,35 @@
         <f>SUM(((S11-S10)/2),S10)</f>
         <v>75.2</v>
       </c>
-      <c r="T19" s="349" t="s">
+      <c r="T19" s="297" t="s">
         <v>61</v>
       </c>
       <c r="U19" s="32"/>
-      <c r="V19" s="350" t="s">
+      <c r="V19" s="298" t="s">
         <v>141</v>
       </c>
       <c r="W19" s="157"/>
-      <c r="X19" s="350" t="s">
+      <c r="X19" s="298" t="s">
         <v>83</v>
       </c>
       <c r="Y19" s="68"/>
-      <c r="Z19" s="350" t="s">
+      <c r="Z19" s="298" t="s">
         <v>83</v>
       </c>
       <c r="AA19" s="68"/>
-      <c r="AB19" s="351" t="s">
+      <c r="AB19" s="299" t="s">
         <v>94</v>
       </c>
       <c r="AC19" s="75"/>
-      <c r="AD19" s="327" t="s">
+      <c r="AD19" s="326" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B20" s="347" t="s">
+      <c r="B20" s="319" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="348"/>
+      <c r="C20" s="320"/>
       <c r="D20" s="20">
         <v>300</v>
       </c>
@@ -4113,33 +4128,33 @@
         <f>SUM(((S10-S12) /2),S12)</f>
         <v>-20.320000000000007</v>
       </c>
-      <c r="T20" s="349" t="s">
+      <c r="T20" s="297" t="s">
         <v>60</v>
       </c>
       <c r="U20" s="33"/>
-      <c r="V20" s="349" t="s">
+      <c r="V20" s="297" t="s">
         <v>140</v>
       </c>
       <c r="W20" s="156"/>
-      <c r="X20" s="349" t="s">
+      <c r="X20" s="297" t="s">
         <v>84</v>
       </c>
       <c r="Y20" s="44"/>
-      <c r="Z20" s="349" t="s">
+      <c r="Z20" s="297" t="s">
         <v>84</v>
       </c>
       <c r="AA20" s="44"/>
-      <c r="AB20" s="351" t="s">
+      <c r="AB20" s="299" t="s">
         <v>95</v>
       </c>
       <c r="AC20" s="76"/>
-      <c r="AD20" s="327"/>
+      <c r="AD20" s="326"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B21" s="298" t="s">
+      <c r="B21" s="321" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="299"/>
+      <c r="C21" s="322"/>
       <c r="D21" s="20">
         <v>180</v>
       </c>
@@ -4194,36 +4209,36 @@
         <f>SUM(((S11-S12)/2),S12)</f>
         <v>-12.339999999999989</v>
       </c>
-      <c r="T21" s="349" t="s">
+      <c r="T21" s="297" t="s">
         <v>59</v>
       </c>
       <c r="U21" s="34"/>
-      <c r="V21" s="308" t="s">
-        <v>151</v>
-      </c>
-      <c r="W21" s="309"/>
-      <c r="X21" s="349" t="s">
+      <c r="V21" s="296" t="s">
+        <v>212</v>
+      </c>
+      <c r="W21" s="357"/>
+      <c r="X21" s="297" t="s">
         <v>85</v>
       </c>
       <c r="Y21" s="45"/>
-      <c r="Z21" s="349" t="s">
+      <c r="Z21" s="297" t="s">
         <v>85</v>
       </c>
       <c r="AA21" s="45"/>
-      <c r="AB21" s="351" t="s">
+      <c r="AB21" s="299" t="s">
         <v>96</v>
       </c>
       <c r="AC21" s="80"/>
-      <c r="AD21" s="327"/>
+      <c r="AD21" s="326"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A22" s="310" t="s">
+      <c r="A22" s="354" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="306" t="s">
+      <c r="B22" s="338" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="307"/>
+      <c r="C22" s="339"/>
       <c r="D22" s="94">
         <v>90</v>
       </c>
@@ -4278,11 +4293,11 @@
         <f>SUM(((S10-S13)/2),S13)</f>
         <v>26.54</v>
       </c>
-      <c r="T22" s="355" t="s">
+      <c r="T22" s="303" t="s">
         <v>66</v>
       </c>
       <c r="U22" s="101"/>
-      <c r="V22" s="355" t="s">
+      <c r="V22" s="303" t="s">
         <v>109</v>
       </c>
       <c r="W22" s="102"/>
@@ -4298,12 +4313,12 @@
         <v>97</v>
       </c>
       <c r="AC22" s="104"/>
-      <c r="AD22" s="327"/>
+      <c r="AD22" s="326"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A23" s="310"/>
-      <c r="B23" s="308"/>
-      <c r="C23" s="309"/>
+      <c r="A23" s="354"/>
+      <c r="B23" s="317"/>
+      <c r="C23" s="318"/>
       <c r="D23" s="105">
         <v>270</v>
       </c>
@@ -4313,38 +4328,38 @@
       <c r="F23" s="107">
         <v>100</v>
       </c>
-      <c r="G23" s="303"/>
-      <c r="H23" s="304"/>
-      <c r="I23" s="311"/>
-      <c r="J23" s="300"/>
-      <c r="K23" s="302"/>
-      <c r="L23" s="302"/>
-      <c r="M23" s="301"/>
-      <c r="N23" s="300"/>
-      <c r="O23" s="302"/>
-      <c r="P23" s="301"/>
-      <c r="Q23" s="303"/>
-      <c r="R23" s="304"/>
-      <c r="S23" s="305"/>
-      <c r="T23" s="354" t="s">
+      <c r="G23" s="308"/>
+      <c r="H23" s="309"/>
+      <c r="I23" s="352"/>
+      <c r="J23" s="306"/>
+      <c r="K23" s="353"/>
+      <c r="L23" s="353"/>
+      <c r="M23" s="307"/>
+      <c r="N23" s="306"/>
+      <c r="O23" s="353"/>
+      <c r="P23" s="307"/>
+      <c r="Q23" s="308"/>
+      <c r="R23" s="309"/>
+      <c r="S23" s="310"/>
+      <c r="T23" s="302" t="s">
         <v>114</v>
       </c>
       <c r="U23" s="109"/>
-      <c r="V23" s="300"/>
-      <c r="W23" s="301"/>
-      <c r="X23" s="300"/>
-      <c r="Y23" s="301"/>
-      <c r="Z23" s="300"/>
-      <c r="AA23" s="301"/>
-      <c r="AB23" s="300"/>
-      <c r="AC23" s="301"/>
-      <c r="AD23" s="327"/>
+      <c r="V23" s="306"/>
+      <c r="W23" s="307"/>
+      <c r="X23" s="306"/>
+      <c r="Y23" s="307"/>
+      <c r="Z23" s="306"/>
+      <c r="AA23" s="307"/>
+      <c r="AB23" s="306"/>
+      <c r="AC23" s="307"/>
+      <c r="AD23" s="326"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B24" s="298" t="s">
+      <c r="B24" s="321" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="299"/>
+      <c r="C24" s="322"/>
       <c r="D24" s="20">
         <v>330</v>
       </c>
@@ -4398,33 +4413,33 @@
         <f>SUM(((S10-S14)/2),S14)</f>
         <v>3.1899999999999977</v>
       </c>
-      <c r="T24" s="349" t="s">
+      <c r="T24" s="297" t="s">
         <v>68</v>
       </c>
       <c r="U24" s="36"/>
-      <c r="V24" s="349" t="s">
+      <c r="V24" s="297" t="s">
         <v>68</v>
       </c>
       <c r="W24" s="36"/>
-      <c r="X24" s="349" t="s">
+      <c r="X24" s="297" t="s">
         <v>68</v>
       </c>
       <c r="Y24" s="36"/>
-      <c r="Z24" s="349" t="s">
+      <c r="Z24" s="297" t="s">
         <v>68</v>
       </c>
       <c r="AA24" s="36"/>
-      <c r="AB24" s="351" t="s">
+      <c r="AB24" s="299" t="s">
         <v>98</v>
       </c>
       <c r="AC24" s="81"/>
-      <c r="AD24" s="327"/>
+      <c r="AD24" s="326"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B25" s="298" t="s">
+      <c r="B25" s="321" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="299"/>
+      <c r="C25" s="322"/>
       <c r="D25" s="20">
         <v>30</v>
       </c>
@@ -4479,33 +4494,33 @@
         <f>SUM(((S10-S15)/2),S15)</f>
         <v>80.849999999999994</v>
       </c>
-      <c r="T25" s="349" t="s">
+      <c r="T25" s="297" t="s">
         <v>69</v>
       </c>
       <c r="U25" s="37"/>
-      <c r="V25" s="349" t="s">
+      <c r="V25" s="297" t="s">
         <v>142</v>
       </c>
       <c r="W25" s="158"/>
-      <c r="X25" s="349" t="s">
+      <c r="X25" s="297" t="s">
         <v>69</v>
       </c>
       <c r="Y25" s="37"/>
-      <c r="Z25" s="349" t="s">
+      <c r="Z25" s="297" t="s">
         <v>69</v>
       </c>
       <c r="AA25" s="37"/>
-      <c r="AB25" s="351" t="s">
+      <c r="AB25" s="299" t="s">
         <v>99</v>
       </c>
       <c r="AC25" s="82"/>
-      <c r="AD25" s="327"/>
+      <c r="AD25" s="326"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B26" s="298" t="s">
+      <c r="B26" s="321" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="299"/>
+      <c r="C26" s="322"/>
       <c r="D26" s="20">
         <v>240</v>
       </c>
@@ -4560,33 +4575,33 @@
         <f>SUM(((S13-S14)/2),S14)</f>
         <v>-37.49</v>
       </c>
-      <c r="T26" s="349" t="s">
+      <c r="T26" s="297" t="s">
         <v>63</v>
       </c>
       <c r="U26" s="38"/>
-      <c r="V26" s="352" t="s">
+      <c r="V26" s="300" t="s">
         <v>110</v>
       </c>
       <c r="W26" s="90"/>
-      <c r="X26" s="349" t="s">
+      <c r="X26" s="297" t="s">
         <v>87</v>
       </c>
       <c r="Y26" s="46"/>
-      <c r="Z26" s="349" t="s">
+      <c r="Z26" s="297" t="s">
         <v>87</v>
       </c>
       <c r="AA26" s="46"/>
-      <c r="AB26" s="349" t="s">
+      <c r="AB26" s="297" t="s">
         <v>100</v>
       </c>
       <c r="AC26" s="83"/>
-      <c r="AD26" s="327"/>
+      <c r="AD26" s="326"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B27" s="298" t="s">
+      <c r="B27" s="321" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="299"/>
+      <c r="C27" s="322"/>
       <c r="D27" s="20">
         <v>0</v>
       </c>
@@ -4640,33 +4655,33 @@
         <f>SUM(((S15-S14)/2),S14)</f>
         <v>16.819999999999993</v>
       </c>
-      <c r="T27" s="349" t="s">
+      <c r="T27" s="297" t="s">
         <v>56</v>
       </c>
       <c r="U27" s="39"/>
-      <c r="V27" s="352" t="s">
+      <c r="V27" s="300" t="s">
         <v>143</v>
       </c>
       <c r="W27" s="159"/>
-      <c r="X27" s="349" t="s">
+      <c r="X27" s="297" t="s">
         <v>88</v>
       </c>
       <c r="Y27" s="47"/>
-      <c r="Z27" s="349" t="s">
+      <c r="Z27" s="297" t="s">
         <v>88</v>
       </c>
       <c r="AA27" s="47"/>
-      <c r="AB27" s="349" t="s">
+      <c r="AB27" s="297" t="s">
         <v>101</v>
       </c>
       <c r="AC27" s="84"/>
-      <c r="AD27" s="327"/>
+      <c r="AD27" s="326"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B28" s="298" t="s">
+      <c r="B28" s="321" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="299"/>
+      <c r="C28" s="322"/>
       <c r="D28" s="20">
         <v>150</v>
       </c>
@@ -4721,36 +4736,36 @@
         <f>SUM(((S11-S13)/2),S13)</f>
         <v>34.520000000000003</v>
       </c>
-      <c r="T28" s="349" t="s">
+      <c r="T28" s="297" t="s">
         <v>64</v>
       </c>
       <c r="U28" s="40"/>
-      <c r="V28" s="352" t="s">
+      <c r="V28" s="300" t="s">
         <v>111</v>
       </c>
       <c r="W28" s="91"/>
-      <c r="X28" s="349" t="s">
+      <c r="X28" s="297" t="s">
         <v>64</v>
       </c>
       <c r="Y28" s="40"/>
-      <c r="Z28" s="349" t="s">
+      <c r="Z28" s="297" t="s">
         <v>64</v>
       </c>
       <c r="AA28" s="40"/>
-      <c r="AB28" s="349" t="s">
+      <c r="AB28" s="297" t="s">
         <v>102</v>
       </c>
       <c r="AC28" s="85"/>
-      <c r="AD28" s="327"/>
+      <c r="AD28" s="326"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A29" s="310" t="s">
+      <c r="A29" s="354" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="306" t="s">
+      <c r="B29" s="338" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="307"/>
+      <c r="C29" s="339"/>
       <c r="D29" s="94">
         <v>210</v>
       </c>
@@ -4804,32 +4819,32 @@
         <f>SUM(((S11-S14)/2),S14)</f>
         <v>11.170000000000002</v>
       </c>
-      <c r="T29" s="355" t="s">
+      <c r="T29" s="303" t="s">
         <v>67</v>
       </c>
       <c r="U29" s="110"/>
-      <c r="V29" s="353" t="s">
+      <c r="V29" s="301" t="s">
         <v>144</v>
       </c>
       <c r="W29" s="160"/>
-      <c r="X29" s="355" t="s">
+      <c r="X29" s="303" t="s">
         <v>86</v>
       </c>
       <c r="Y29" s="103"/>
-      <c r="Z29" s="355" t="s">
+      <c r="Z29" s="303" t="s">
         <v>86</v>
       </c>
       <c r="AA29" s="103"/>
-      <c r="AB29" s="355" t="s">
+      <c r="AB29" s="303" t="s">
         <v>103</v>
       </c>
       <c r="AC29" s="111"/>
-      <c r="AD29" s="327"/>
+      <c r="AD29" s="326"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A30" s="310"/>
-      <c r="B30" s="308"/>
-      <c r="C30" s="309"/>
+      <c r="A30" s="354"/>
+      <c r="B30" s="317"/>
+      <c r="C30" s="318"/>
       <c r="D30" s="105">
         <v>30</v>
       </c>
@@ -4839,38 +4854,38 @@
       <c r="F30" s="107">
         <v>100</v>
       </c>
-      <c r="G30" s="303"/>
-      <c r="H30" s="304"/>
-      <c r="I30" s="311"/>
-      <c r="J30" s="300"/>
-      <c r="K30" s="302"/>
-      <c r="L30" s="302"/>
-      <c r="M30" s="301"/>
-      <c r="N30" s="300"/>
-      <c r="O30" s="302"/>
-      <c r="P30" s="301"/>
-      <c r="Q30" s="303"/>
-      <c r="R30" s="304"/>
-      <c r="S30" s="305"/>
-      <c r="T30" s="354" t="s">
+      <c r="G30" s="308"/>
+      <c r="H30" s="309"/>
+      <c r="I30" s="352"/>
+      <c r="J30" s="306"/>
+      <c r="K30" s="353"/>
+      <c r="L30" s="353"/>
+      <c r="M30" s="307"/>
+      <c r="N30" s="306"/>
+      <c r="O30" s="353"/>
+      <c r="P30" s="307"/>
+      <c r="Q30" s="308"/>
+      <c r="R30" s="309"/>
+      <c r="S30" s="310"/>
+      <c r="T30" s="302" t="s">
         <v>115</v>
       </c>
       <c r="U30" s="112"/>
-      <c r="V30" s="300"/>
-      <c r="W30" s="301"/>
-      <c r="X30" s="300"/>
-      <c r="Y30" s="301"/>
-      <c r="Z30" s="300"/>
-      <c r="AA30" s="301"/>
-      <c r="AB30" s="300"/>
-      <c r="AC30" s="301"/>
-      <c r="AD30" s="327"/>
+      <c r="V30" s="306"/>
+      <c r="W30" s="307"/>
+      <c r="X30" s="306"/>
+      <c r="Y30" s="307"/>
+      <c r="Z30" s="306"/>
+      <c r="AA30" s="307"/>
+      <c r="AB30" s="306"/>
+      <c r="AC30" s="307"/>
+      <c r="AD30" s="326"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B31" s="298" t="s">
+      <c r="B31" s="321" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="299"/>
+      <c r="C31" s="322"/>
       <c r="D31" s="20">
         <v>90</v>
       </c>
@@ -4925,37 +4940,37 @@
         <f>SUM(((S15-S11)/2),S11)</f>
         <v>88.830000000000013</v>
       </c>
-      <c r="T31" s="349" t="s">
+      <c r="T31" s="297" t="s">
         <v>66</v>
       </c>
       <c r="U31" s="35"/>
-      <c r="V31" s="352" t="s">
+      <c r="V31" s="300" t="s">
         <v>145</v>
       </c>
       <c r="W31" s="161"/>
-      <c r="X31" s="349" t="s">
+      <c r="X31" s="297" t="s">
         <v>66</v>
       </c>
       <c r="Y31" s="35"/>
-      <c r="Z31" s="349" t="s">
+      <c r="Z31" s="297" t="s">
         <v>66</v>
       </c>
       <c r="AA31" s="35"/>
-      <c r="AB31" s="349" t="s">
+      <c r="AB31" s="297" t="s">
         <v>104</v>
       </c>
       <c r="AC31" s="86"/>
-      <c r="AD31" s="327"/>
-      <c r="AH31" s="316" t="s">
+      <c r="AD31" s="326"/>
+      <c r="AH31" s="337" t="s">
         <v>93</v>
       </c>
-      <c r="AI31" s="316"/>
+      <c r="AI31" s="337"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B32" s="298" t="s">
+      <c r="B32" s="321" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="299"/>
+      <c r="C32" s="322"/>
       <c r="D32" s="20">
         <v>210</v>
       </c>
@@ -5010,33 +5025,33 @@
         <f>SUM(((S13-S12)/2),S12)</f>
         <v>-61</v>
       </c>
-      <c r="T32" s="349" t="s">
+      <c r="T32" s="297" t="s">
         <v>67</v>
       </c>
       <c r="U32" s="41"/>
-      <c r="V32" s="352" t="s">
+      <c r="V32" s="300" t="s">
         <v>112</v>
       </c>
       <c r="W32" s="92"/>
-      <c r="X32" s="349" t="s">
+      <c r="X32" s="297" t="s">
         <v>67</v>
       </c>
       <c r="Y32" s="41"/>
-      <c r="Z32" s="349" t="s">
+      <c r="Z32" s="297" t="s">
         <v>67</v>
       </c>
       <c r="AA32" s="41"/>
-      <c r="AB32" s="349" t="s">
+      <c r="AB32" s="297" t="s">
         <v>105</v>
       </c>
       <c r="AC32" s="87"/>
-      <c r="AD32" s="327"/>
+      <c r="AD32" s="326"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B33" s="298" t="s">
+      <c r="B33" s="321" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="299"/>
+      <c r="C33" s="322"/>
       <c r="D33" s="20">
         <v>270</v>
       </c>
@@ -5091,36 +5106,36 @@
         <f>SUM(((S14-S12)/2),S12)</f>
         <v>-84.35</v>
       </c>
-      <c r="T33" s="349" t="s">
+      <c r="T33" s="297" t="s">
         <v>65</v>
       </c>
       <c r="U33" s="42"/>
-      <c r="V33" s="352" t="s">
+      <c r="V33" s="300" t="s">
         <v>146</v>
       </c>
       <c r="W33" s="162"/>
-      <c r="X33" s="349" t="s">
+      <c r="X33" s="297" t="s">
         <v>65</v>
       </c>
       <c r="Y33" s="42"/>
-      <c r="Z33" s="349" t="s">
+      <c r="Z33" s="297" t="s">
         <v>65</v>
       </c>
       <c r="AA33" s="42"/>
-      <c r="AB33" s="349" t="s">
+      <c r="AB33" s="297" t="s">
         <v>106</v>
       </c>
       <c r="AC33" s="88"/>
-      <c r="AD33" s="327"/>
+      <c r="AD33" s="326"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A34" s="310" t="s">
+      <c r="A34" s="354" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="306" t="s">
+      <c r="B34" s="338" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="307"/>
+      <c r="C34" s="339"/>
       <c r="D34" s="94">
         <v>150</v>
       </c>
@@ -5174,19 +5189,19 @@
         <f>SUM(((S15-S12)/2),S12)</f>
         <v>-6.6899999999999977</v>
       </c>
-      <c r="T34" s="355" t="s">
+      <c r="T34" s="303" t="s">
         <v>64</v>
       </c>
       <c r="U34" s="113"/>
-      <c r="V34" s="353" t="s">
+      <c r="V34" s="301" t="s">
         <v>147</v>
       </c>
       <c r="W34" s="163"/>
-      <c r="X34" s="355" t="s">
+      <c r="X34" s="303" t="s">
         <v>86</v>
       </c>
       <c r="Y34" s="103"/>
-      <c r="Z34" s="355" t="s">
+      <c r="Z34" s="303" t="s">
         <v>86</v>
       </c>
       <c r="AA34" s="103"/>
@@ -5194,12 +5209,12 @@
         <v>107</v>
       </c>
       <c r="AC34" s="114"/>
-      <c r="AD34" s="327"/>
+      <c r="AD34" s="326"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A35" s="310"/>
-      <c r="B35" s="308"/>
-      <c r="C35" s="309"/>
+      <c r="A35" s="354"/>
+      <c r="B35" s="317"/>
+      <c r="C35" s="318"/>
       <c r="D35" s="105">
         <v>330</v>
       </c>
@@ -5209,38 +5224,38 @@
       <c r="F35" s="107">
         <v>100</v>
       </c>
-      <c r="G35" s="303"/>
-      <c r="H35" s="304"/>
-      <c r="I35" s="311"/>
-      <c r="J35" s="300"/>
-      <c r="K35" s="302"/>
-      <c r="L35" s="302"/>
-      <c r="M35" s="301"/>
-      <c r="N35" s="300"/>
-      <c r="O35" s="302"/>
-      <c r="P35" s="301"/>
-      <c r="Q35" s="303"/>
-      <c r="R35" s="304"/>
-      <c r="S35" s="305"/>
-      <c r="T35" s="354" t="s">
+      <c r="G35" s="308"/>
+      <c r="H35" s="309"/>
+      <c r="I35" s="352"/>
+      <c r="J35" s="306"/>
+      <c r="K35" s="353"/>
+      <c r="L35" s="353"/>
+      <c r="M35" s="307"/>
+      <c r="N35" s="306"/>
+      <c r="O35" s="353"/>
+      <c r="P35" s="307"/>
+      <c r="Q35" s="308"/>
+      <c r="R35" s="309"/>
+      <c r="S35" s="310"/>
+      <c r="T35" s="302" t="s">
         <v>117</v>
       </c>
       <c r="U35" s="115"/>
-      <c r="V35" s="300"/>
-      <c r="W35" s="301"/>
-      <c r="X35" s="300"/>
-      <c r="Y35" s="301"/>
-      <c r="Z35" s="300"/>
-      <c r="AA35" s="301"/>
-      <c r="AB35" s="300"/>
-      <c r="AC35" s="301"/>
-      <c r="AD35" s="327"/>
+      <c r="V35" s="306"/>
+      <c r="W35" s="307"/>
+      <c r="X35" s="306"/>
+      <c r="Y35" s="307"/>
+      <c r="Z35" s="306"/>
+      <c r="AA35" s="307"/>
+      <c r="AB35" s="306"/>
+      <c r="AC35" s="307"/>
+      <c r="AD35" s="326"/>
     </row>
     <row r="36" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="298" t="s">
+      <c r="B36" s="321" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="299"/>
+      <c r="C36" s="322"/>
       <c r="D36" s="20">
         <v>120</v>
       </c>
@@ -5295,67 +5310,67 @@
         <f>SUM(((S15-S13)/2),S13)</f>
         <v>40.17</v>
       </c>
-      <c r="T36" s="349" t="s">
+      <c r="T36" s="297" t="s">
         <v>70</v>
       </c>
       <c r="U36" s="43"/>
-      <c r="V36" s="352" t="s">
+      <c r="V36" s="300" t="s">
         <v>113</v>
       </c>
       <c r="W36" s="93"/>
-      <c r="X36" s="349" t="s">
+      <c r="X36" s="297" t="s">
         <v>89</v>
       </c>
       <c r="Y36" s="48"/>
-      <c r="Z36" s="349" t="s">
+      <c r="Z36" s="297" t="s">
         <v>89</v>
       </c>
       <c r="AA36" s="48"/>
-      <c r="AB36" s="349" t="s">
+      <c r="AB36" s="297" t="s">
         <v>108</v>
       </c>
       <c r="AC36" s="89"/>
-      <c r="AD36" s="327"/>
+      <c r="AD36" s="326"/>
     </row>
     <row r="37" spans="1:30" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="345" t="s">
+      <c r="B37" s="315" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="346"/>
-      <c r="D37" s="346"/>
-      <c r="E37" s="346"/>
-      <c r="F37" s="346"/>
-      <c r="G37" s="346"/>
-      <c r="H37" s="346"/>
-      <c r="I37" s="346"/>
-      <c r="J37" s="346"/>
-      <c r="K37" s="346"/>
-      <c r="L37" s="346"/>
-      <c r="M37" s="346"/>
-      <c r="N37" s="346"/>
-      <c r="O37" s="346"/>
-      <c r="P37" s="346"/>
-      <c r="Q37" s="346"/>
-      <c r="R37" s="346"/>
-      <c r="S37" s="346"/>
-      <c r="T37" s="346"/>
-      <c r="U37" s="346"/>
-      <c r="V37" s="346"/>
-      <c r="W37" s="346"/>
-      <c r="X37" s="346"/>
-      <c r="Y37" s="346"/>
-      <c r="Z37" s="346"/>
-      <c r="AA37" s="346"/>
-      <c r="AB37" s="346"/>
-      <c r="AC37" s="346"/>
+      <c r="C37" s="316"/>
+      <c r="D37" s="316"/>
+      <c r="E37" s="316"/>
+      <c r="F37" s="316"/>
+      <c r="G37" s="316"/>
+      <c r="H37" s="316"/>
+      <c r="I37" s="316"/>
+      <c r="J37" s="316"/>
+      <c r="K37" s="316"/>
+      <c r="L37" s="316"/>
+      <c r="M37" s="316"/>
+      <c r="N37" s="316"/>
+      <c r="O37" s="316"/>
+      <c r="P37" s="316"/>
+      <c r="Q37" s="316"/>
+      <c r="R37" s="316"/>
+      <c r="S37" s="316"/>
+      <c r="T37" s="316"/>
+      <c r="U37" s="316"/>
+      <c r="V37" s="316"/>
+      <c r="W37" s="316"/>
+      <c r="X37" s="316"/>
+      <c r="Y37" s="316"/>
+      <c r="Z37" s="316"/>
+      <c r="AA37" s="316"/>
+      <c r="AB37" s="316"/>
+      <c r="AC37" s="316"/>
       <c r="AD37" s="28"/>
     </row>
     <row r="38" spans="1:30" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="258"/>
-      <c r="B38" s="312" t="s">
+      <c r="B38" s="348" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="313"/>
+      <c r="C38" s="349"/>
       <c r="D38" s="177">
         <f>SUM(((D19-D12)/2),D12)</f>
         <v>150</v>
@@ -5439,16 +5454,16 @@
         <v>206</v>
       </c>
       <c r="AC38" s="269"/>
-      <c r="AD38" s="327" t="s">
+      <c r="AD38" s="326" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="258"/>
-      <c r="B39" s="298" t="s">
+      <c r="B39" s="321" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="299"/>
+      <c r="C39" s="322"/>
       <c r="D39" s="120">
         <f>SUM(((D20-D11)/2),D11)</f>
         <v>210</v>
@@ -5532,14 +5547,14 @@
         <v>207</v>
       </c>
       <c r="AC39" s="270"/>
-      <c r="AD39" s="327"/>
+      <c r="AD39" s="326"/>
     </row>
     <row r="40" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="258"/>
-      <c r="B40" s="314" t="s">
+      <c r="B40" s="350" t="s">
         <v>192</v>
       </c>
-      <c r="C40" s="315"/>
+      <c r="C40" s="351"/>
       <c r="D40" s="118">
         <f>SUM(((D21-D10)/2),D10)</f>
         <v>90</v>
@@ -5607,10 +5622,10 @@
         <v>66</v>
       </c>
       <c r="U40" s="35"/>
-      <c r="V40" s="296" t="s">
+      <c r="V40" s="355" t="s">
         <v>151</v>
       </c>
-      <c r="W40" s="297"/>
+      <c r="W40" s="356"/>
       <c r="X40" s="244" t="s">
         <v>202</v>
       </c>
@@ -5623,14 +5638,14 @@
         <v>208</v>
       </c>
       <c r="AC40" s="271"/>
-      <c r="AD40" s="327"/>
+      <c r="AD40" s="326"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="231"/>
-      <c r="B41" s="306" t="s">
+      <c r="B41" s="338" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="307"/>
+      <c r="C41" s="339"/>
       <c r="D41" s="94">
         <f>SUM(((D24-D12)/2),D12)</f>
         <v>285</v>
@@ -5714,14 +5729,14 @@
         <v>136</v>
       </c>
       <c r="AC41" s="150"/>
-      <c r="AD41" s="327"/>
+      <c r="AD41" s="326"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="231"/>
-      <c r="B42" s="298" t="s">
+      <c r="B42" s="321" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="299"/>
+      <c r="C42" s="322"/>
       <c r="D42" s="71">
         <f>SUM(((D20-D14)/2),D14)</f>
         <v>300</v>
@@ -5806,14 +5821,14 @@
         <v>137</v>
       </c>
       <c r="AC42" s="152"/>
-      <c r="AD42" s="327"/>
+      <c r="AD42" s="326"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="231"/>
-      <c r="B43" s="308" t="s">
+      <c r="B43" s="317" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="309"/>
+      <c r="C43" s="318"/>
       <c r="D43" s="105">
         <f>SUM(((D33-D10)/2),D10)</f>
         <v>135</v>
@@ -5897,14 +5912,14 @@
         <v>138</v>
       </c>
       <c r="AC43" s="154"/>
-      <c r="AD43" s="327"/>
+      <c r="AD43" s="326"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="231"/>
-      <c r="B44" s="306" t="s">
+      <c r="B44" s="338" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="307"/>
+      <c r="C44" s="339"/>
       <c r="D44" s="94">
         <f t="shared" ref="D44:I44" si="9">SUM(((D12-D28)/2),D28)</f>
         <v>195</v>
@@ -5973,10 +5988,10 @@
         <v>149</v>
       </c>
       <c r="U44" s="165"/>
-      <c r="V44" s="306" t="s">
+      <c r="V44" s="338" t="s">
         <v>151</v>
       </c>
-      <c r="W44" s="307"/>
+      <c r="W44" s="339"/>
       <c r="X44" s="116" t="s">
         <v>153</v>
       </c>
@@ -5989,14 +6004,14 @@
         <v>156</v>
       </c>
       <c r="AC44" s="174"/>
-      <c r="AD44" s="327"/>
+      <c r="AD44" s="326"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="231"/>
-      <c r="B45" s="298" t="s">
+      <c r="B45" s="321" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="299"/>
+      <c r="C45" s="322"/>
       <c r="D45" s="71">
         <f>SUM(((D32-D11)/2),D11)</f>
         <v>165</v>
@@ -6081,14 +6096,14 @@
         <v>157</v>
       </c>
       <c r="AC45" s="175"/>
-      <c r="AD45" s="327"/>
+      <c r="AD45" s="326"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="231"/>
-      <c r="B46" s="308" t="s">
+      <c r="B46" s="317" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="309"/>
+      <c r="C46" s="318"/>
       <c r="D46" s="105">
         <f>SUM(((D21-D13)/2),D13)</f>
         <v>180</v>
@@ -6157,10 +6172,10 @@
         <v>59</v>
       </c>
       <c r="U46" s="167"/>
-      <c r="V46" s="308" t="s">
+      <c r="V46" s="317" t="s">
         <v>151</v>
       </c>
-      <c r="W46" s="309"/>
+      <c r="W46" s="318"/>
       <c r="X46" s="118" t="s">
         <v>155</v>
       </c>
@@ -6173,14 +6188,14 @@
         <v>158</v>
       </c>
       <c r="AC46" s="176"/>
-      <c r="AD46" s="327"/>
+      <c r="AD46" s="326"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="258"/>
-      <c r="B47" s="306" t="s">
+      <c r="B47" s="338" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="307"/>
+      <c r="C47" s="339"/>
       <c r="D47" s="116">
         <f>SUM(((D26-D15)/2),D15)</f>
         <v>150</v>
@@ -6265,14 +6280,14 @@
         <v>209</v>
       </c>
       <c r="AC47" s="272"/>
-      <c r="AD47" s="327"/>
+      <c r="AD47" s="326"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="258"/>
-      <c r="B48" s="298" t="s">
+      <c r="B48" s="321" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="299"/>
+      <c r="C48" s="322"/>
       <c r="D48" s="120">
         <f>SUM(((D36-D14)/2),D14)</f>
         <v>210</v>
@@ -6341,10 +6356,10 @@
         <v>67</v>
       </c>
       <c r="U48" s="41"/>
-      <c r="V48" s="298" t="s">
+      <c r="V48" s="321" t="s">
         <v>151</v>
       </c>
-      <c r="W48" s="299"/>
+      <c r="W48" s="322"/>
       <c r="X48" s="120" t="s">
         <v>204</v>
       </c>
@@ -6357,14 +6372,14 @@
         <v>210</v>
       </c>
       <c r="AC48" s="273"/>
-      <c r="AD48" s="327"/>
+      <c r="AD48" s="326"/>
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" s="258"/>
-      <c r="B49" s="308" t="s">
+      <c r="B49" s="317" t="s">
         <v>194</v>
       </c>
-      <c r="C49" s="309"/>
+      <c r="C49" s="318"/>
       <c r="D49" s="118">
         <f>SUM(((D27-D13)/2),D13)</f>
         <v>90</v>
@@ -6449,13 +6464,13 @@
         <v>211</v>
       </c>
       <c r="AC49" s="274"/>
-      <c r="AD49" s="327"/>
+      <c r="AD49" s="326"/>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B50" s="306" t="s">
+      <c r="B50" s="338" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="307"/>
+      <c r="C50" s="339"/>
       <c r="D50" s="94">
         <f>SUM(((D26-D12)/2),D12)</f>
         <v>240</v>
@@ -6524,10 +6539,10 @@
         <v>63</v>
       </c>
       <c r="U50" s="198"/>
-      <c r="V50" s="306" t="s">
+      <c r="V50" s="338" t="s">
         <v>151</v>
       </c>
-      <c r="W50" s="307"/>
+      <c r="W50" s="339"/>
       <c r="X50" s="116" t="s">
         <v>171</v>
       </c>
@@ -6540,13 +6555,13 @@
         <v>180</v>
       </c>
       <c r="AC50" s="221"/>
-      <c r="AD50" s="327"/>
+      <c r="AD50" s="326"/>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B51" s="298" t="s">
+      <c r="B51" s="321" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="299"/>
+      <c r="C51" s="322"/>
       <c r="D51" s="71">
         <f>SUM(((D14-D32)/2),D32)</f>
         <v>255</v>
@@ -6615,10 +6630,10 @@
         <v>159</v>
       </c>
       <c r="U51" s="199"/>
-      <c r="V51" s="298" t="s">
+      <c r="V51" s="321" t="s">
         <v>151</v>
       </c>
-      <c r="W51" s="299"/>
+      <c r="W51" s="322"/>
       <c r="X51" s="120" t="s">
         <v>172</v>
       </c>
@@ -6631,13 +6646,13 @@
         <v>181</v>
       </c>
       <c r="AC51" s="222"/>
-      <c r="AD51" s="327"/>
+      <c r="AD51" s="326"/>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B52" s="308" t="s">
+      <c r="B52" s="317" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="309"/>
+      <c r="C52" s="318"/>
       <c r="D52" s="105">
         <f>SUM(((D33-D13)/2),D13)</f>
         <v>225</v>
@@ -6706,10 +6721,10 @@
         <v>160</v>
       </c>
       <c r="U52" s="200"/>
-      <c r="V52" s="308" t="s">
+      <c r="V52" s="317" t="s">
         <v>151</v>
       </c>
-      <c r="W52" s="309"/>
+      <c r="W52" s="318"/>
       <c r="X52" s="118" t="s">
         <v>173</v>
       </c>
@@ -6722,13 +6737,13 @@
         <v>182</v>
       </c>
       <c r="AC52" s="223"/>
-      <c r="AD52" s="327"/>
+      <c r="AD52" s="326"/>
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B53" s="306" t="s">
+      <c r="B53" s="338" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="307"/>
+      <c r="C53" s="339"/>
       <c r="D53" s="131">
         <f>SUM(((D28-D15)/2),D15)</f>
         <v>105</v>
@@ -6813,16 +6828,16 @@
         <v>183</v>
       </c>
       <c r="AC53" s="224"/>
-      <c r="AD53" s="327"/>
+      <c r="AD53" s="326"/>
       <c r="AI53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B54" s="298" t="s">
+      <c r="B54" s="321" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="299"/>
+      <c r="C54" s="322"/>
       <c r="D54" s="133">
         <f>SUM(((D36-D11)/2),D11)</f>
         <v>120</v>
@@ -6907,13 +6922,13 @@
         <v>184</v>
       </c>
       <c r="AC54" s="225"/>
-      <c r="AD54" s="327"/>
+      <c r="AD54" s="326"/>
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B55" s="308" t="s">
+      <c r="B55" s="317" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="309"/>
+      <c r="C55" s="318"/>
       <c r="D55" s="135">
         <f>SUM(((D13-D31)/2),D31)</f>
         <v>135</v>
@@ -6998,13 +7013,13 @@
         <v>185</v>
       </c>
       <c r="AC55" s="226"/>
-      <c r="AD55" s="327"/>
+      <c r="AD55" s="326"/>
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B56" s="306" t="s">
+      <c r="B56" s="338" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="307"/>
+      <c r="C56" s="339"/>
       <c r="D56" s="131">
         <v>15</v>
       </c>
@@ -7088,13 +7103,13 @@
         <v>186</v>
       </c>
       <c r="AC56" s="227"/>
-      <c r="AD56" s="327"/>
+      <c r="AD56" s="326"/>
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B57" s="298" t="s">
+      <c r="B57" s="321" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="299"/>
+      <c r="C57" s="322"/>
       <c r="D57" s="133">
         <v>345</v>
       </c>
@@ -7177,13 +7192,13 @@
         <v>187</v>
       </c>
       <c r="AC57" s="228"/>
-      <c r="AD57" s="327"/>
+      <c r="AD57" s="326"/>
     </row>
     <row r="58" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="328" t="s">
+      <c r="B58" s="340" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="329"/>
+      <c r="C58" s="341"/>
       <c r="D58" s="188">
         <f>SUM(((D27-D10)/2),D10)</f>
         <v>0</v>
@@ -7268,37 +7283,84 @@
         <v>188</v>
       </c>
       <c r="AC58" s="229"/>
-      <c r="AD58" s="327"/>
+      <c r="AD58" s="326"/>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="G60" s="326" t="s">
+      <c r="G60" s="336" t="s">
         <v>122</v>
       </c>
-      <c r="H60" s="326"/>
-      <c r="I60" s="326"/>
-      <c r="J60" s="326"/>
-      <c r="K60" s="326"/>
-      <c r="L60" s="326"/>
-      <c r="M60" s="326"/>
+      <c r="H60" s="336"/>
+      <c r="I60" s="336"/>
+      <c r="J60" s="336"/>
+      <c r="K60" s="336"/>
+      <c r="L60" s="336"/>
+      <c r="M60" s="336"/>
     </row>
   </sheetData>
-  <mergeCells count="95">
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B37:AC37"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
+  <mergeCells count="94">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="V40:W40"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="G60:M60"/>
+    <mergeCell ref="AH31:AI31"/>
+    <mergeCell ref="AD38:AD58"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="V51:W51"/>
+    <mergeCell ref="V52:W52"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="V50:W50"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="T17:AC17"/>
     <mergeCell ref="AD19:AD36"/>
     <mergeCell ref="J17:M17"/>
@@ -7315,69 +7377,21 @@
     <mergeCell ref="V30:W30"/>
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="G60:M60"/>
-    <mergeCell ref="AH31:AI31"/>
-    <mergeCell ref="AD38:AD58"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="V51:W51"/>
-    <mergeCell ref="V52:W52"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="V50:W50"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="V40:W40"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="AB35:AC35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B37:AC37"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8705,8 +8719,8 @@
       <c r="Z20" s="13"/>
       <c r="AA20" s="283"/>
       <c r="AB20" s="284"/>
-      <c r="AF20" s="316"/>
-      <c r="AG20" s="316"/>
+      <c r="AF20" s="337"/>
+      <c r="AG20" s="337"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="291" t="s">

</xml_diff>